<commit_message>
Inserido dados da linha Água Verde no BD.
</commit_message>
<xml_diff>
--- a/Repositorio/BD/GeradorJSON.xlsx
+++ b/Repositorio/BD/GeradorJSON.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCC\Repositorio\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97658E02-4BBB-4C16-B51B-CB6ACC221DF9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0A5F2C-0C97-407D-86E6-36BF1689A110}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="1" activeTab="3" xr2:uid="{A9038219-B9CF-4E97-BE7C-F60600EF4568}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="1" activeTab="2" xr2:uid="{A9038219-B9CF-4E97-BE7C-F60600EF4568}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="LinhaPonto" sheetId="3" r:id="rId3"/>
-    <sheet name="HoraPonto" sheetId="4" r:id="rId4"/>
+    <sheet name="horaLinha" sheetId="3" r:id="rId3"/>
+    <sheet name="horaLinhaPonto" sheetId="4" r:id="rId4"/>
     <sheet name="Ponto" sheetId="5" r:id="rId5"/>
+    <sheet name="linhas" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179021" calcMode="manual"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="251">
   <si>
     <t>Semana</t>
   </si>
@@ -558,21 +559,6 @@
     <t>19:30</t>
   </si>
   <si>
-    <t>Ponto A</t>
-  </si>
-  <si>
-    <t>Ponto B</t>
-  </si>
-  <si>
-    <t>Ponto C</t>
-  </si>
-  <si>
-    <t>Ponto D</t>
-  </si>
-  <si>
-    <t>Ponto E</t>
-  </si>
-  <si>
     <t>Ponto 1</t>
   </si>
   <si>
@@ -598,13 +584,217 @@
   </si>
   <si>
     <t>Ponto 9</t>
+  </si>
+  <si>
+    <t>são os horários do site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">é a sequencia de pontos que a linha segue. </t>
+  </si>
+  <si>
+    <t>devemos inserir os sentidos</t>
+  </si>
+  <si>
+    <t>resultado</t>
+  </si>
+  <si>
+    <t>SentidoPonto</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Praça</t>
+  </si>
+  <si>
+    <t>Bairro Água Verde</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>SentidoLinha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrição </t>
+  </si>
+  <si>
+    <t>Bairro</t>
+  </si>
+  <si>
+    <t>Ponto virtual</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>Ponto 10</t>
+  </si>
+  <si>
+    <t>Ponto 11</t>
+  </si>
+  <si>
+    <t>Ponto 12</t>
+  </si>
+  <si>
+    <t>Ponto 13</t>
+  </si>
+  <si>
+    <t>Ponto 14</t>
+  </si>
+  <si>
+    <t>Ponto 15</t>
+  </si>
+  <si>
+    <t>Ponto 16</t>
+  </si>
+  <si>
+    <t>Ponto 17</t>
+  </si>
+  <si>
+    <t>Ponto 18</t>
+  </si>
+  <si>
+    <t>Ponto 19</t>
+  </si>
+  <si>
+    <t>Ponto 20</t>
+  </si>
+  <si>
+    <t>IFSC</t>
+  </si>
+  <si>
+    <t>Endereço</t>
+  </si>
+  <si>
+    <t>V. Guilherme Prust</t>
+  </si>
+  <si>
+    <t>Praça Lauro Mueller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Av. Expedicionários </t>
+  </si>
+  <si>
+    <t>R. Alvino Voigt</t>
+  </si>
+  <si>
+    <t>R. Jacobe Scheuer</t>
+  </si>
+  <si>
+    <t>Lateral SC280</t>
+  </si>
+  <si>
+    <t>R. Mario Maier</t>
+  </si>
+  <si>
+    <t>R. Jacobe Fuck</t>
+  </si>
+  <si>
+    <t>R. Sergio Gapski</t>
+  </si>
+  <si>
+    <t>(Sem nome)</t>
+  </si>
+  <si>
+    <t>Ponto Físico</t>
+  </si>
+  <si>
+    <t>Ponto 21</t>
+  </si>
+  <si>
+    <t>Ponto 22</t>
+  </si>
+  <si>
+    <t>Ponto 23</t>
+  </si>
+  <si>
+    <t>Ponto 24</t>
+  </si>
+  <si>
+    <t>Ponto 25</t>
+  </si>
+  <si>
+    <t>Ponto 26</t>
+  </si>
+  <si>
+    <t>Ponto 27</t>
+  </si>
+  <si>
+    <t>Ponto 28</t>
+  </si>
+  <si>
+    <t>Ponto 29</t>
+  </si>
+  <si>
+    <t>Ponto 30</t>
+  </si>
+  <si>
+    <t>Ponto 31</t>
+  </si>
+  <si>
+    <t>Ponto 32</t>
+  </si>
+  <si>
+    <t>Ponto 33</t>
+  </si>
+  <si>
+    <t>Ponto 34</t>
+  </si>
+  <si>
+    <t>R. Antonio Grosskopf</t>
+  </si>
+  <si>
+    <t>R. Narciso Ruthes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Último ponto antes do retorno para a praça. </t>
+  </si>
+  <si>
+    <t>Ponto virtual, próximo ao Procopiak</t>
+  </si>
+  <si>
+    <t>Ponto 35</t>
+  </si>
+  <si>
+    <t>Ponto virtual. Próximo ao posto Guapo.</t>
+  </si>
+  <si>
+    <t>R. Fracisco de Paula Pereira</t>
+  </si>
+  <si>
+    <t>Ponto virtual.</t>
+  </si>
+  <si>
+    <t>Ponto virtual. Próx. retifica Motocar</t>
+  </si>
+  <si>
+    <t>Ponto Físico. Próximo da Escola Estadual Emília Ferrero</t>
+  </si>
+  <si>
+    <t>Inicio da linha.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ponto final. </t>
+  </si>
+  <si>
+    <t>RoteiroPontos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, Ponto 25, Ponto 26, Ponto 27, Ponto 28, Ponto 29, Ponto 30, Ponto 31, Ponto 32, Ponto 33, Ponto 34, Ponto 35, </t>
+  </si>
+  <si>
+    <t>Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, Ponto 25, Ponto 26, Ponto 27, Ponto 28, Ponto 29, Ponto 30, Ponto 31, Ponto 32, Ponto 33, Ponto 34, Ponto 35</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -643,6 +833,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF777777"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -816,7 +1019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1026,6 +1229,33 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2150,16 +2380,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>103909</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>116032</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>416873</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>88818</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>236405</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>20199</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2536011</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>183485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2182,8 +2412,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17772784" y="3164032"/>
-          <a:ext cx="6838096" cy="4666667"/>
+          <a:off x="4553444" y="11899818"/>
+          <a:ext cx="6868031" cy="4666667"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2199,15 +2429,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>24</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>103909</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>116032</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>236405</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>20199</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4100,10 +4330,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76005D01-6542-4084-AE0C-F52B6237E75C}">
-  <dimension ref="F14:P143"/>
+  <dimension ref="F12:P143"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="I62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K110" sqref="K110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4121,6 +4351,11 @@
     <col min="17" max="16384" width="9.140625" style="70"/>
   </cols>
   <sheetData>
+    <row r="12" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F12" s="72" t="s">
+        <v>183</v>
+      </c>
+    </row>
     <row r="14" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F14" s="1" t="s">
         <v>104</v>
@@ -7079,30 +7314,50 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10646AB-5585-46AB-8FFD-FBA1CD63180D}">
-  <dimension ref="F14:O24"/>
+  <dimension ref="C10:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="B10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="70"/>
-    <col min="6" max="6" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="27.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" style="70" customWidth="1"/>
-    <col min="11" max="11" width="2.42578125" style="70" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" style="70" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="2.28515625" style="70" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.42578125" style="70" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="70"/>
+    <col min="3" max="3" width="43.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="76" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="74.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="70" customWidth="1"/>
+    <col min="11" max="11" width="2" style="70" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.140625" style="70" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="2" style="70" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="70"/>
   </cols>
   <sheetData>
-    <row r="14" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F14" s="1" t="s">
-        <v>104</v>
-      </c>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="72" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="72" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I13" s="1" t="str">
+        <f>$N$14&amp;$L$14&amp;$H15&amp;$L$14&amp;$M$14&amp;$L$14&amp;$H16&amp;$L$14</f>
+        <v>,"Intervalo":"0"</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
       <c r="K14" s="70" t="s">
         <v>109</v>
       </c>
@@ -7119,180 +7374,891 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F15" s="1" t="s">
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="D15" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="E15" s="26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F15" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="G15" s="77" t="s">
+        <v>188</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="70" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>174</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I16" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G16" s="76" t="s">
+        <v>246</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="70" t="str">
+        <f>K$14&amp;L$14&amp;C$15&amp;L$14&amp;M$14&amp;L$14&amp;C16&amp;L$14&amp;N$14&amp;L$14&amp;D$15&amp;L$14&amp;M$14&amp;L$14&amp;D16&amp;L$14&amp;N$14&amp;L$14&amp;$F$15&amp;L$14&amp;M$14&amp;L$14&amp;$F16&amp;L$14&amp;N$14&amp;L$14&amp;E$15&amp;L$14&amp;M$14&amp;L$14&amp;E16&amp;L$14&amp;$N$14&amp;$L$14&amp;$G$15&amp;$L$14&amp;$M$14&amp;$L$14&amp;$G16&amp;$L$14&amp;$N$14&amp;$L$14&amp;$H$15&amp;$L$14&amp;$M$14&amp;$L$14&amp;$H16&amp;$L$14&amp;O$14&amp;N$14</f>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 1","Descrição":"Inicio da linha.","Intervalo":"0"},</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G17" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I17" s="70" t="str">
+        <f t="shared" ref="I17:I51" si="0">K$14&amp;L$14&amp;C$15&amp;L$14&amp;M$14&amp;L$14&amp;C17&amp;L$14&amp;N$14&amp;L$14&amp;D$15&amp;L$14&amp;M$14&amp;L$14&amp;D17&amp;L$14&amp;N$14&amp;L$14&amp;$F$15&amp;L$14&amp;M$14&amp;L$14&amp;$F17&amp;L$14&amp;N$14&amp;L$14&amp;E$15&amp;L$14&amp;M$14&amp;L$14&amp;E17&amp;L$14&amp;$N$14&amp;$L$14&amp;$G$15&amp;$L$14&amp;$M$14&amp;$L$14&amp;$G17&amp;$L$14&amp;$N$14&amp;$L$14&amp;$H$15&amp;$L$14&amp;$M$14&amp;$L$14&amp;$H17&amp;$L$14&amp;O$14&amp;N$14</f>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 2","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G18" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I18" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 3","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G19" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I19" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 4","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I20" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 5","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G21" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I21" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 6","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G22" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I22" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 7","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G23" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I23" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 8","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G24" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I24" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 9","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G25" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I25" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 10","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G26" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I26" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 11","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G27" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I27" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 12","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G28" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I28" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 13","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G29" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I29" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 14","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G30" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I30" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 15","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G31" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I31" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 16","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G32" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I32" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 17","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G33" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I33" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 18","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G34" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I34" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 19","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G35" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I35" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 20","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G36" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="I36" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 21","Descrição":"-","Intervalo":"1.6"},</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G37" s="76" t="s">
+        <v>238</v>
+      </c>
+      <c r="H37" s="1">
+        <v>2</v>
+      </c>
+      <c r="I37" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Bairro Água Verde","PontoID":"Ponto 22","Descrição":"Último ponto antes do retorno para a praça. ","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G38" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" s="1">
+        <v>2</v>
+      </c>
+      <c r="I38" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 23","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G39" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H39" s="1">
+        <v>2</v>
+      </c>
+      <c r="I39" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 24","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G40" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H40" s="1">
+        <v>2</v>
+      </c>
+      <c r="I40" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 25","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G41" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H41" s="1">
+        <v>2</v>
+      </c>
+      <c r="I41" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 26","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G42" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H42" s="1">
+        <v>2</v>
+      </c>
+      <c r="I42" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 27","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G43" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H43" s="1">
+        <v>2</v>
+      </c>
+      <c r="I43" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 28","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G44" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H44" s="1">
+        <v>2</v>
+      </c>
+      <c r="I44" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 29","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G45" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H45" s="1">
+        <v>2</v>
+      </c>
+      <c r="I45" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 30","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G46" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H46" s="1">
+        <v>2</v>
+      </c>
+      <c r="I46" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 31","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G47" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47" s="1">
+        <v>2</v>
+      </c>
+      <c r="I47" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 32","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G48" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H48" s="1">
+        <v>2</v>
+      </c>
+      <c r="I48" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 33","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G49" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H49" s="1">
+        <v>2</v>
+      </c>
+      <c r="I49" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 34","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C50" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G50" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="H50" s="1">
+        <v>2</v>
+      </c>
+      <c r="I50" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 35","Descrição":"-","Intervalo":"2"},</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="J16" s="70" t="str">
-        <f>K$14&amp;L$14&amp;F$15&amp;L$14&amp;M$14&amp;L$14&amp;F16&amp;L$14&amp;N$14&amp;L$14&amp;G$15&amp;L$14&amp;M$14&amp;L$14&amp;G16&amp;L$14&amp;N$14&amp;L$14&amp;H$15&amp;L$14&amp;M$14&amp;L$14&amp;H16&amp;L$14&amp;N$14&amp;L$14&amp;I$15&amp;L$14&amp;M$14&amp;L$14&amp;I16&amp;L$14&amp;O$14&amp;N$14</f>
-        <v>{"LinhaID":"Cohab II","RoteiroInicio":"Terminal Urbano","RoteiroFim":"Bairro Cohab II","PontoID":"Ponto A"},</v>
-      </c>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F17" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="J17" s="70" t="str">
-        <f t="shared" ref="J17:J24" si="0">K$14&amp;L$14&amp;F$15&amp;L$14&amp;M$14&amp;L$14&amp;F17&amp;L$14&amp;N$14&amp;L$14&amp;G$15&amp;L$14&amp;M$14&amp;L$14&amp;G17&amp;L$14&amp;N$14&amp;L$14&amp;H$15&amp;L$14&amp;M$14&amp;L$14&amp;H17&amp;L$14&amp;N$14&amp;L$14&amp;I$15&amp;L$14&amp;M$14&amp;L$14&amp;I17&amp;L$14&amp;O$14&amp;N$14</f>
-        <v>{"LinhaID":"Cohab II","RoteiroInicio":"Terminal Urbano","RoteiroFim":"Bairro Cohab II","PontoID":"Ponto C"},</v>
-      </c>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F18" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="J18" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Cohab II","RoteiroInicio":"Terminal Urbano","RoteiroFim":"Bairro Cohab II","PontoID":"Ponto D"},</v>
-      </c>
-    </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F19" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J19" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Cohab II","RoteiroInicio":"Terminal Urbano","RoteiroFim":"Bairro Cohab II","PontoID":"Ponto B"},</v>
-      </c>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F20" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="J20" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Cohab II","RoteiroInicio":"Terminal Urbano","RoteiroFim":"Bairro Cohab II","PontoID":"Ponto E"},</v>
-      </c>
-    </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F21" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="J21" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Cohab I","RoteiroInicio":"Terminal Urbano","RoteiroFim":"Bairro Cohab I","PontoID":"Ponto E"},</v>
-      </c>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F22" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="J22" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Cohab I","RoteiroInicio":"Terminal Urbano","RoteiroFim":"Bairro Cohab I","PontoID":"Ponto D"},</v>
-      </c>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="J23" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Cohab I","RoteiroInicio":"Terminal Urbano","RoteiroFim":"Bairro Cohab I","PontoID":"Ponto C"},</v>
-      </c>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J24" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Cohab I","RoteiroInicio":"Terminal Urbano","RoteiroFim":"Bairro Cohab I","PontoID":"Ponto B"},</v>
+      <c r="F51" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G51" s="76" t="s">
+        <v>247</v>
+      </c>
+      <c r="H51" s="1">
+        <v>2</v>
+      </c>
+      <c r="I51" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"LinhaID":"Campo Água Verde","RoteiroInicio":"Praça","SentidoLinha":"Praça Lauro Mueller","PontoID":"Ponto 1","Descrição":"Ponto final. ","Intervalo":"2"},</v>
       </c>
     </row>
   </sheetData>
@@ -7303,225 +8269,1390 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{924C03B5-9AE1-4FC4-AF7D-985FA0BA2472}">
-  <dimension ref="F14:O24"/>
+  <dimension ref="B3:M44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="70"/>
-    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="100.5703125" style="70" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" style="70" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.85546875" style="70" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="1.5703125" style="70" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="1.7109375" style="70" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="70"/>
+    <col min="1" max="1" width="9.140625" style="70"/>
+    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="78" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="76" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.5703125" style="70" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" style="70" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="1.5703125" style="70" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" style="70" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="70"/>
   </cols>
   <sheetData>
-    <row r="14" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F14" s="1" t="s">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C3" s="1">
+        <v>-26.18674</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-50.360370000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C4" s="75"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K14" s="70" t="s">
+      <c r="I8" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="L14" s="70" t="s">
+      <c r="J8" s="70" t="s">
         <v>113</v>
       </c>
-      <c r="M14" s="70" t="s">
+      <c r="K8" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="N14" s="70" t="s">
+      <c r="L8" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="O14" s="70" t="s">
+      <c r="M8" s="70" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F15" s="1" t="s">
-        <v>11</v>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="F9" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="H9" s="74" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-26.17371</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-50.390079999999998</v>
+      </c>
+      <c r="E10" s="78" t="s">
+        <v>212</v>
+      </c>
+      <c r="F10" s="76" t="s">
+        <v>212</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H10" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B10&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C10&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D10&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F10&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G10&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 1","Latitude":"-26.17371","Longitude":"-50.39008","Descrição ":"Praça Lauro Mueller","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-26.17314</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-50.388159999999999</v>
+      </c>
+      <c r="E11" s="78" t="s">
+        <v>242</v>
+      </c>
+      <c r="F11" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H11" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B11&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C11&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D11&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F11&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G11&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 2","Latitude":"-26.17314","Longitude":"-50.38816","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-26.17154</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-50.38456</v>
+      </c>
+      <c r="E12" s="78" t="s">
+        <v>211</v>
+      </c>
+      <c r="F12" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H12" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B12&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C12&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D12&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F12&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G12&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 3","Latitude":"-26.17154","Longitude":"-50.38456","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-26.173500000000001</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-50.37932</v>
+      </c>
+      <c r="E13" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H13" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B13&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C13&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D13&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F13&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G13&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 4","Latitude":"-26.1735","Longitude":"-50.37932","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-26.176279999999998</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-50.37574</v>
+      </c>
+      <c r="E14" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="F14" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H14" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B14&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C14&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D14&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F14&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G14&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 5","Latitude":"-26.17628","Longitude":"-50.37574","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-26.180530000000001</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-50.370330000000003</v>
+      </c>
+      <c r="E15" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="F15" s="76" t="s">
+        <v>196</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F16" s="1" t="s">
-        <v>179</v>
+        <v>195</v>
+      </c>
+      <c r="H15" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B15&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C15&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D15&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F15&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G15&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 6","Latitude":"-26.18053","Longitude":"-50.37033","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-26.183009999999999</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-50.367199999999997</v>
+      </c>
+      <c r="E16" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="F16" s="76" t="s">
+        <v>209</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="J16" s="70" t="str">
-        <f>K$14&amp;L$14&amp;F$15&amp;L$14&amp;M$14&amp;L$14&amp;F16&amp;L$14&amp;N$14&amp;L$14&amp;G$15&amp;L$14&amp;M$14&amp;L$14&amp;G16&amp;L$14&amp;N$14&amp;L$14&amp;H$15&amp;L$14&amp;M$14&amp;L$14&amp;H16&amp;L$14&amp;N$14&amp;L$14&amp;I$15&amp;L$14&amp;M$14&amp;L$14&amp;I16&amp;L$14&amp;O$14&amp;N$14</f>
-        <v>{"LinhaID":"Ponto 1","Ponto":"Terminal Urbano","RoteiroFim":"Bairro Cohab II","PontoID":"Ponto A"},</v>
-      </c>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F17" s="1" t="s">
-        <v>180</v>
+        <v>195</v>
+      </c>
+      <c r="H16" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B16&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C16&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D16&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F16&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G16&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 7","Latitude":"-26.18301","Longitude":"-50.3672","Descrição ":"IFSC","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-26.18411</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-50.362879999999997</v>
+      </c>
+      <c r="E17" s="78" t="s">
+        <v>214</v>
+      </c>
+      <c r="F17" s="76" t="s">
+        <v>196</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="J17" s="70" t="str">
-        <f t="shared" ref="J17:J24" si="0">K$14&amp;L$14&amp;F$15&amp;L$14&amp;M$14&amp;L$14&amp;F17&amp;L$14&amp;N$14&amp;L$14&amp;G$15&amp;L$14&amp;M$14&amp;L$14&amp;G17&amp;L$14&amp;N$14&amp;L$14&amp;H$15&amp;L$14&amp;M$14&amp;L$14&amp;H17&amp;L$14&amp;N$14&amp;L$14&amp;I$15&amp;L$14&amp;M$14&amp;L$14&amp;I17&amp;L$14&amp;O$14&amp;N$14</f>
-        <v>{"LinhaID":"Ponto 2","Ponto":"Terminal Urbano","RoteiroFim":"Bairro Cohab II","PontoID":"Ponto C"},</v>
-      </c>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F18" s="1" t="s">
-        <v>181</v>
+        <v>195</v>
+      </c>
+      <c r="H17" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B17&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C17&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D17&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F17&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G17&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 8","Latitude":"-26.18411","Longitude":"-50.36288","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-26.18573</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-50.360770000000002</v>
+      </c>
+      <c r="E18" s="78" t="s">
+        <v>214</v>
+      </c>
+      <c r="F18" s="76" t="s">
+        <v>196</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="J18" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Ponto 3","Ponto":"Terminal Urbano","RoteiroFim":"Bairro Cohab II","PontoID":"Ponto D"},</v>
-      </c>
-    </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F19" s="1" t="s">
-        <v>182</v>
+        <v>195</v>
+      </c>
+      <c r="H18" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B18&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C18&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D18&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F18&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G18&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 9","Latitude":"-26.18573","Longitude":"-50.36077","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19" s="1">
+        <v>-26.18674</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-50.360370000000003</v>
+      </c>
+      <c r="E19" s="78" t="s">
+        <v>215</v>
+      </c>
+      <c r="F19" s="76" t="s">
+        <v>196</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J19" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Ponto 4","Ponto":"Terminal Urbano","RoteiroFim":"Bairro Cohab II","PontoID":"Ponto B"},</v>
-      </c>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F20" s="1" t="s">
-        <v>183</v>
+        <v>195</v>
+      </c>
+      <c r="H19" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B19&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C19&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D19&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F19&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G19&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 10","Latitude":"-26.18674","Longitude":"-50.36037","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C20" s="1">
+        <v>-26.18796</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-50.364640000000001</v>
+      </c>
+      <c r="E20" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="F20" s="76" t="s">
+        <v>196</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="J20" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Ponto 5","Ponto":"Terminal Urbano","RoteiroFim":"Bairro Cohab II","PontoID":"Ponto E"},</v>
-      </c>
-    </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F21" s="1" t="s">
-        <v>184</v>
+        <v>195</v>
+      </c>
+      <c r="H20" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B20&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C20&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D20&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F20&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G20&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 11","Latitude":"-26.18796","Longitude":"-50.36464","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C21" s="1">
+        <v>-26.188690000000001</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-50.368810000000003</v>
+      </c>
+      <c r="E21" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="F21" s="76" t="s">
+        <v>196</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="J21" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Ponto 6","Ponto":"Terminal Urbano","RoteiroFim":"Bairro Cohab I","PontoID":"Ponto E"},</v>
-      </c>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F22" s="1" t="s">
-        <v>185</v>
+        <v>195</v>
+      </c>
+      <c r="H21" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B21&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C21&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D21&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F21&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G21&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 12","Latitude":"-26.18869","Longitude":"-50.36881","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-26.189419999999998</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-50.373460000000001</v>
+      </c>
+      <c r="E22" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="F22" s="76" t="s">
+        <v>244</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="J22" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Ponto 7","Ponto":"Terminal Urbano","RoteiroFim":"Bairro Cohab I","PontoID":"Ponto D"},</v>
-      </c>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F23" s="1" t="s">
-        <v>186</v>
+        <v>195</v>
+      </c>
+      <c r="H22" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B22&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C22&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D22&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F22&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G22&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 13","Latitude":"-26.18942","Longitude":"-50.37346","Descrição ":"Ponto virtual. Próx. retifica Motocar","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C23" s="1">
+        <v>-26.1907</v>
+      </c>
+      <c r="D23" s="1">
+        <v>-50.378329999999998</v>
+      </c>
+      <c r="E23" s="78" t="s">
+        <v>217</v>
+      </c>
+      <c r="F23" s="76" t="s">
+        <v>196</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="J23" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Ponto 8","Ponto":"Terminal Urbano","RoteiroFim":"Bairro Cohab I","PontoID":"Ponto C"},</v>
-      </c>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="1" t="s">
-        <v>187</v>
+        <v>195</v>
+      </c>
+      <c r="H23" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B23&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C23&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D23&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F23&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G23&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 14","Latitude":"-26.1907","Longitude":"-50.37833","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C24" s="1">
+        <v>-26.19408</v>
+      </c>
+      <c r="D24" s="1">
+        <v>-50.378</v>
+      </c>
+      <c r="E24" s="78" t="s">
+        <v>218</v>
+      </c>
+      <c r="F24" s="76" t="s">
+        <v>196</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J24" s="70" t="str">
-        <f t="shared" si="0"/>
-        <v>{"LinhaID":"Ponto 9","Ponto":"Terminal Urbano","RoteiroFim":"Bairro Cohab I","PontoID":"Ponto B"},</v>
+        <v>195</v>
+      </c>
+      <c r="H24" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B24&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C24&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D24&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F24&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G24&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 15","Latitude":"-26.19408","Longitude":"-50.378","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" s="1">
+        <v>-26.195879999999999</v>
+      </c>
+      <c r="D25" s="1">
+        <v>-50.378239999999998</v>
+      </c>
+      <c r="E25" s="78" t="s">
+        <v>219</v>
+      </c>
+      <c r="F25" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H25" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B25&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C25&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D25&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F25&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G25&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 16","Latitude":"-26.19588","Longitude":"-50.37824","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C26" s="1">
+        <v>-26.199590000000001</v>
+      </c>
+      <c r="D26" s="1">
+        <v>-50.37876</v>
+      </c>
+      <c r="E26" s="78" t="s">
+        <v>220</v>
+      </c>
+      <c r="F26" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H26" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B26&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C26&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D26&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F26&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G26&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 17","Latitude":"-26.19959","Longitude":"-50.37876","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C27" s="1">
+        <v>-26.201070000000001</v>
+      </c>
+      <c r="D27" s="1">
+        <v>-50.382820000000002</v>
+      </c>
+      <c r="E27" s="78" t="s">
+        <v>220</v>
+      </c>
+      <c r="F27" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H27" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B27&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C27&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D27&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F27&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G27&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 18","Latitude":"-26.20107","Longitude":"-50.38282","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" s="1">
+        <v>-26.203022000000001</v>
+      </c>
+      <c r="D28" s="1">
+        <v>-50.384556000000003</v>
+      </c>
+      <c r="E28" s="78" t="s">
+        <v>220</v>
+      </c>
+      <c r="F28" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H28" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B28&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C28&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D28&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F28&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G28&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 19","Latitude":"-26.203022","Longitude":"-50.384556","Descrição ":"Ponto Físico","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="1">
+        <v>-26.205335999999999</v>
+      </c>
+      <c r="D29" s="1">
+        <v>-50.383465000000001</v>
+      </c>
+      <c r="E29" s="78" t="s">
+        <v>220</v>
+      </c>
+      <c r="F29" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H29" s="70" t="str">
+        <f>I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B29&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C29&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D29&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F29&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G29&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 20","Latitude":"-26.205336","Longitude":"-50.383465","Descrição ":"Ponto Físico","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" s="1">
+        <v>-26.20448</v>
+      </c>
+      <c r="D30" s="1">
+        <v>-50.379910000000002</v>
+      </c>
+      <c r="E30" s="78" t="s">
+        <v>236</v>
+      </c>
+      <c r="F30" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H30" s="70" t="str">
+        <f t="shared" ref="H30:H44" si="0">I$8&amp;J$8&amp;B$9&amp;J$8&amp;K$8&amp;J$8&amp;B30&amp;J$8&amp;L$8&amp;J$8&amp;C$9&amp;J$8&amp;K$8&amp;J$8&amp;C30&amp;J$8&amp;L$8&amp;J$8&amp;D$9&amp;J$8&amp;K$8&amp;J$8&amp;D30&amp;J$8&amp;L$8&amp;J$8&amp;F$9&amp;J$8&amp;K$8&amp;J$8&amp;F30&amp;J$8&amp;$L$8&amp;$J$8&amp;$G$9&amp;$J$8&amp;$K$8&amp;$J$8&amp;G30&amp;$J$8&amp;M$8&amp;L$8</f>
+        <v>{"PontoID":"Ponto 21","Latitude":"-26.20448","Longitude":"-50.37991","Descrição ":"Ponto virtual","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C31" s="1">
+        <v>-26.200403000000001</v>
+      </c>
+      <c r="D31" s="1">
+        <v>-50.376750000000001</v>
+      </c>
+      <c r="E31" s="78" t="s">
+        <v>237</v>
+      </c>
+      <c r="F31" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H31" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 22","Latitude":"-26.200403","Longitude":"-50.37675","Descrição ":"Ponto Físico","SentidoPonto":"Bairro"},</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C32" s="1">
+        <v>-26.197900000000001</v>
+      </c>
+      <c r="D32" s="1">
+        <v>-50.377719999999997</v>
+      </c>
+      <c r="E32" s="78" t="s">
+        <v>219</v>
+      </c>
+      <c r="F32" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H32" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 23","Latitude":"-26.1979","Longitude":"-50.37772","Descrição ":"Ponto virtual","SentidoPonto":"Praça"},</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C33" s="1">
+        <v>-26.193760000000001</v>
+      </c>
+      <c r="D33" s="1">
+        <v>-50.377130000000001</v>
+      </c>
+      <c r="E33" s="78" t="s">
+        <v>218</v>
+      </c>
+      <c r="F33" s="76" t="s">
+        <v>245</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H33" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 24","Latitude":"-26.19376","Longitude":"-50.37713","Descrição ":"Ponto Físico. Próximo da Escola Estadual Emília Ferrero","SentidoPonto":"Praça"},</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C34" s="1">
+        <v>-26.190619999999999</v>
+      </c>
+      <c r="D34" s="1">
+        <v>-50.378320000000002</v>
+      </c>
+      <c r="E34" s="78" t="s">
+        <v>217</v>
+      </c>
+      <c r="F34" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H34" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 25","Latitude":"-26.19062","Longitude":"-50.37832","Descrição ":"Ponto virtual","SentidoPonto":"Praça"},</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C35" s="1">
+        <v>-26.18956</v>
+      </c>
+      <c r="D35" s="1">
+        <v>-50.372929999999997</v>
+      </c>
+      <c r="E35" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="F35" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H35" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 26","Latitude":"-26.18956","Longitude":"-50.37293","Descrição ":"Ponto virtual","SentidoPonto":"Praça"},</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C36" s="1">
+        <v>-26.188179999999999</v>
+      </c>
+      <c r="D36" s="1">
+        <v>-50.364379999999997</v>
+      </c>
+      <c r="E36" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="F36" s="76" t="s">
+        <v>239</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H36" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 27","Latitude":"-26.18818","Longitude":"-50.36438","Descrição ":"Ponto virtual, próximo ao Procopiak","SentidoPonto":"Praça"},</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" s="1">
+        <v>-26.18422</v>
+      </c>
+      <c r="D37" s="1">
+        <v>-50.36262</v>
+      </c>
+      <c r="E37" s="78" t="s">
+        <v>214</v>
+      </c>
+      <c r="F37" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H37" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 28","Latitude":"-26.18422","Longitude":"-50.36262","Descrição ":"Ponto Físico","SentidoPonto":"Praça"},</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C38" s="1">
+        <v>-26.18318</v>
+      </c>
+      <c r="D38" s="1">
+        <v>-50.366849999999999</v>
+      </c>
+      <c r="E38" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="F38" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H38" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 29","Latitude":"-26.18318","Longitude":"-50.36685","Descrição ":"Ponto Físico","SentidoPonto":"Praça"},</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C39" s="1">
+        <v>-26.181576</v>
+      </c>
+      <c r="D39" s="1">
+        <v>-50.369019999999999</v>
+      </c>
+      <c r="E39" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="F39" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H39" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 30","Latitude":"-26.181576","Longitude":"-50.36902","Descrição ":"Ponto Físico","SentidoPonto":"Praça"},</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C40" s="1">
+        <v>-26.179175999999998</v>
+      </c>
+      <c r="D40" s="1">
+        <v>-50.371997999999998</v>
+      </c>
+      <c r="E40" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="F40" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H40" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 31","Latitude":"-26.179176","Longitude":"-50.371998","Descrição ":"Ponto Físico","SentidoPonto":"Praça"},</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C41" s="1">
+        <v>-26.176902999999999</v>
+      </c>
+      <c r="D41" s="1">
+        <v>-50.374890000000001</v>
+      </c>
+      <c r="E41" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="F41" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H41" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 32","Latitude":"-26.176903","Longitude":"-50.37489","Descrição ":"Ponto Físico","SentidoPonto":"Praça"},</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" s="1">
+        <v>-26.173763000000001</v>
+      </c>
+      <c r="D42" s="1">
+        <v>-50.378974999999997</v>
+      </c>
+      <c r="E42" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="F42" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H42" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 33","Latitude":"-26.173763","Longitude":"-50.378975","Descrição ":"Ponto Físico","SentidoPonto":"Praça"},</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" s="1">
+        <v>-26.17144</v>
+      </c>
+      <c r="D43" s="1">
+        <v>-50.38373</v>
+      </c>
+      <c r="E43" s="78" t="s">
+        <v>242</v>
+      </c>
+      <c r="F43" s="76" t="s">
+        <v>241</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H43" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 34","Latitude":"-26.17144","Longitude":"-50.38373","Descrição ":"Ponto virtual. Próximo ao posto Guapo.","SentidoPonto":"Praça"},</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C44" s="1">
+        <v>-26.172239999999999</v>
+      </c>
+      <c r="D44" s="1">
+        <v>-50.387230000000002</v>
+      </c>
+      <c r="E44" s="78" t="s">
+        <v>242</v>
+      </c>
+      <c r="F44" s="76" t="s">
+        <v>243</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H44" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PontoID":"Ponto 35","Latitude":"-26.17224","Longitude":"-50.38723","Descrição ":"Ponto virtual.","SentidoPonto":"Praça"},</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7480796-5F2B-4F5A-B934-29D55A666AB2}">
+  <dimension ref="E5:AN46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="5:40" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="5:40" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>248</v>
+      </c>
+      <c r="F6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="5:40" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="5:40" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>174</v>
+      </c>
+      <c r="G11" t="s">
+        <v>175</v>
+      </c>
+      <c r="H11" t="s">
+        <v>176</v>
+      </c>
+      <c r="I11" t="s">
+        <v>177</v>
+      </c>
+      <c r="J11" t="s">
+        <v>178</v>
+      </c>
+      <c r="K11" t="s">
+        <v>179</v>
+      </c>
+      <c r="L11" t="s">
+        <v>180</v>
+      </c>
+      <c r="M11" t="s">
+        <v>181</v>
+      </c>
+      <c r="N11" t="s">
+        <v>182</v>
+      </c>
+      <c r="O11" t="s">
+        <v>198</v>
+      </c>
+      <c r="P11" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>200</v>
+      </c>
+      <c r="R11" t="s">
+        <v>201</v>
+      </c>
+      <c r="S11" t="s">
+        <v>202</v>
+      </c>
+      <c r="T11" t="s">
+        <v>203</v>
+      </c>
+      <c r="U11" t="s">
+        <v>204</v>
+      </c>
+      <c r="V11" t="s">
+        <v>205</v>
+      </c>
+      <c r="W11" t="s">
+        <v>206</v>
+      </c>
+      <c r="X11" t="s">
+        <v>207</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>226</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>227</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>230</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>231</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>232</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>233</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>234</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>235</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="5:40" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F12" s="80" t="str">
+        <f>F11&amp;F10&amp;" "</f>
+        <v xml:space="preserve">Ponto 1, </v>
+      </c>
+      <c r="G12" t="str">
+        <f>F12&amp;G11&amp;$F$10&amp;" "</f>
+        <v xml:space="preserve">Ponto 1, Ponto 2, </v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" ref="H12:AN12" si="0">G12&amp;H11&amp;$F$10&amp;" "</f>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, </v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, </v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, </v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, </v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, </v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, </v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, </v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, </v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, </v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, </v>
+      </c>
+      <c r="R12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, </v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, </v>
+      </c>
+      <c r="T12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, </v>
+      </c>
+      <c r="U12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, </v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, </v>
+      </c>
+      <c r="W12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, </v>
+      </c>
+      <c r="X12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, </v>
+      </c>
+      <c r="Y12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, </v>
+      </c>
+      <c r="Z12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, </v>
+      </c>
+      <c r="AA12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, </v>
+      </c>
+      <c r="AB12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, </v>
+      </c>
+      <c r="AC12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, </v>
+      </c>
+      <c r="AD12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, Ponto 25, </v>
+      </c>
+      <c r="AE12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, Ponto 25, Ponto 26, </v>
+      </c>
+      <c r="AF12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, Ponto 25, Ponto 26, Ponto 27, </v>
+      </c>
+      <c r="AG12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, Ponto 25, Ponto 26, Ponto 27, Ponto 28, </v>
+      </c>
+      <c r="AH12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, Ponto 25, Ponto 26, Ponto 27, Ponto 28, Ponto 29, </v>
+      </c>
+      <c r="AI12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, Ponto 25, Ponto 26, Ponto 27, Ponto 28, Ponto 29, Ponto 30, </v>
+      </c>
+      <c r="AJ12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, Ponto 25, Ponto 26, Ponto 27, Ponto 28, Ponto 29, Ponto 30, Ponto 31, </v>
+      </c>
+      <c r="AK12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, Ponto 25, Ponto 26, Ponto 27, Ponto 28, Ponto 29, Ponto 30, Ponto 31, Ponto 32, </v>
+      </c>
+      <c r="AL12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, Ponto 25, Ponto 26, Ponto 27, Ponto 28, Ponto 29, Ponto 30, Ponto 31, Ponto 32, Ponto 33, </v>
+      </c>
+      <c r="AM12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, Ponto 4, Ponto 5, Ponto 6, Ponto 7, Ponto 8, Ponto 9, Ponto 10, Ponto 11, Ponto 12, Ponto 13, Ponto 14, Ponto 15, Ponto 16, Ponto 17, Ponto 18, Ponto 19, Ponto 20, Ponto 21, Ponto 22, Ponto 23, Ponto 24, Ponto 25, Ponto 26, Ponto 27, Ponto 28, Ponto 29, Ponto 30, Ponto 31, Ponto 32, Ponto 33, Ponto 34, </v>
+      </c>
+      <c r="AN12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="5:40" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="5:40" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>176</v>
+      </c>
+      <c r="H14" t="str">
+        <f>H12</f>
+        <v xml:space="preserve">Ponto 1, Ponto 2, Ponto 3, </v>
+      </c>
+    </row>
+    <row r="15" spans="5:40" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="5:40" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>